<commit_message>
Change to current version of costs.xlsx (old version added originally by accident)
</commit_message>
<xml_diff>
--- a/schematic/costs.xlsx
+++ b/schematic/costs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Component</t>
   </si>
@@ -37,6 +37,30 @@
     <t>Bulk price</t>
   </si>
   <si>
+    <t>schottkey diode</t>
+  </si>
+  <si>
+    <t>http://ca.mouser.com/Search/ProductDetail.aspx?R=BAT54WS-E3-18virtualkey61370000virtualkey78-BAT54WS-E3-18</t>
+  </si>
+  <si>
+    <t>for charge pump</t>
+  </si>
+  <si>
+    <t>2.2microf capacitor</t>
+  </si>
+  <si>
+    <t>2 for charge pump, 1 for connection between VCOMH and VSS for screen</t>
+  </si>
+  <si>
+    <t>530kohm resistor</t>
+  </si>
+  <si>
+    <t>http://ca.mouser.com/ProductDetail/KOA-Speer/RN73H2BTTD5303F100/?qs=sGAEpiMZZMtlubZbdhIBIFiJHX02PtB%2f179V6qep8S8%3d</t>
+  </si>
+  <si>
+    <t>for display circuit iref thing CAUTION IS PACKAGE TOO SMALL?</t>
+  </si>
+  <si>
     <t>attiny84</t>
   </si>
   <si>
@@ -49,31 +73,46 @@
     <t>http://ca.mouser.com/ProductDetail/Analog-Devices/AD8546ARMZ/?qs=sGAEpiMZZMvtNjJQt4UgLalm6EXZly%2fyUbyp8TEAGcc%3d</t>
   </si>
   <si>
-    <t>light diode</t>
-  </si>
-  <si>
-    <t>http://ca.mouser.com/ProductDetail/Vishay-Semiconductors/VEMD2523SLX01/?qs=5csRq1wdUj7%252bW4Twulhzmw==</t>
-  </si>
-  <si>
-    <t>56.2 kOhm resistor</t>
-  </si>
-  <si>
-    <t>http://ca.mouser.com/ProductDetail/TE-Connectivity-Neohm/YR1B56K2CC/?qs=sGAEpiMZZMu61qfTUdNhG7ul34ib6LOjL6bUnrtuVyw%3d</t>
+    <t>photodiode</t>
+  </si>
+  <si>
+    <t>http://ca.mouser.com/ProductDetail/OSRAM-Opto-Semiconductors/BPW-21/?qs=sGAEpiMZZMsgSGrx0WqTbJ5%2fxrVssRlA</t>
+  </si>
+  <si>
+    <t>124 kOhm resistor</t>
+  </si>
+  <si>
+    <t>http://ca.mouser.com/ProductDetail/Yageo/RT1206BRD07124KL/?qs=sGAEpiMZZMtlubZbdhIBIAik%252bt0yKDKekRRw38WH8Bw%3d</t>
   </si>
   <si>
     <t>For specifying op amp gain</t>
   </si>
   <si>
+    <t>200kOhm resistor</t>
+  </si>
+  <si>
+    <t>http://ca.mouser.com/ProductDetail/Vishay/TNPW1206200KBEEA/?qs=sGAEpiMZZMtlubZbdhIBIF8%252bFeqY9QKZaCRqqFGHW0s%3d</t>
+  </si>
+  <si>
+    <t>op amp gain</t>
+  </si>
+  <si>
     <t>0.1microF capacitor</t>
   </si>
   <si>
     <t>http://ca.mouser.com/ProductDetail/Kemet/C412C104K5R5TA/?qs=sGAEpiMZZMsh%252b1woXyUXjyBlPk63JI1iK8zyV%2f0xdlY%3d</t>
   </si>
   <si>
-    <t>High pass filters for photodiodes</t>
-  </si>
-  <si>
-    <t>battery CR2025</t>
+    <t>One as high-pass filter for photodiode; another for charge pump output stabilization</t>
+  </si>
+  <si>
+    <t>battery CR2032</t>
+  </si>
+  <si>
+    <t>battery holder</t>
+  </si>
+  <si>
+    <t>http://ca.mouser.com/ProductDetail/Linx-Technologies/BAT-HLD-001/?qs=sGAEpiMZZMsgSGrx0WqTbEGDMV4VNa3N</t>
   </si>
   <si>
     <t>screen</t>
@@ -85,49 +124,49 @@
     <t>http://ca.mouser.com/ProductDetail/NXP-Semiconductors/2N7002P215/?qs=sGAEpiMZZMvplms98TlKY1Xl2WGfghYYYk%2fNHxw35Uo%3d</t>
   </si>
   <si>
-    <t>Used for switching additional resistors into diode circuit to increase op amp gain in low light.</t>
-  </si>
-  <si>
-    <t>4.7V voltage regulator</t>
-  </si>
-  <si>
-    <t>http://ca.mouser.com/ProductDetail/Texas-Instruments/LP3985IM5-47-NOPB/?qs=sGAEpiMZZMsGz1a6aV8DcBojudwDyMGaeOKXWCPSmoo%3d</t>
-  </si>
-  <si>
-    <t>for AVR power supply (needs at least 4.5V to run at 16MHz, and it has to run at 16MHz for USB library to work)</t>
-  </si>
-  <si>
-    <t>2.2 micro F capacitor</t>
-  </si>
-  <si>
-    <t>http://ca.mouser.com/ProductDetail/Murata-Electronics/GCM31CR71H225KA55L/?qs=sGAEpiMZZMuMW9TJLBQkXuf1BniCIJClUmIgmBULTRc%3d</t>
-  </si>
-  <si>
-    <t>for voltage regulator</t>
-  </si>
-  <si>
-    <t>0.091 micro F capacitor</t>
-  </si>
-  <si>
-    <t>http://ca.mouser.com/ProductDetail/Murata-Electronics/GRM31C5C1H913JA01L/?qs=sGAEpiMZZMs0AnBnWHyRQCxvYDcCBBVRwiw4rH9ae6Q%3d</t>
-  </si>
-  <si>
-    <t>1.5kohm resistor</t>
-  </si>
-  <si>
-    <t>http://ca.mouser.com/ProductDetail/KOA-Speer/MF1-4DC1501F/?qs=sGAEpiMZZMu61qfTUdNhG2%252byzAc6g0mP29BhHAmiV5s%3d</t>
-  </si>
-  <si>
-    <t>usb d- pulldown resistor</t>
-  </si>
-  <si>
-    <t>68 ohm resistor</t>
-  </si>
-  <si>
-    <t>http://ca.mouser.com/ProductDetail/KOA-Speer/MF1-4DC68R0F/?qs=sGAEpiMZZMu61qfTUdNhG2r2Nmyl%2fOMiVUQaBvEclw4%3d</t>
-  </si>
-  <si>
-    <t>usb d+ and d- resistors</t>
+    <t>Used for switching additional resistors into diode circuit to increase op amp gain in low light and for buttons. 3 for op amp, 4 for buttons.</t>
+  </si>
+  <si>
+    <t>2.8V voltage regulator</t>
+  </si>
+  <si>
+    <t>http://ca.mouser.com/ProductDetail/Texas-Instruments/LP5907MFX-33-NOPB/?qs=sGAEpiMZZMtOXy69nW9rM70jJqWEZ9aJwn%2fC2hzxT3w%3d</t>
+  </si>
+  <si>
+    <t>for regulating battery power for everything except screen</t>
+  </si>
+  <si>
+    <t>1 micro F capacitor</t>
+  </si>
+  <si>
+    <t>http://ca.mouser.com/ProductDetail/Vishay-Vitramon/VJ1206Y105MXJTW1BC/?qs=sGAEpiMZZMsh%252b1woXyUXj9C8nVWPqMcew5XpGSaKDds%3d</t>
+  </si>
+  <si>
+    <t>2 for voltage regulator and 1 for op amp</t>
+  </si>
+  <si>
+    <t>0.1 micro F capacitor</t>
+  </si>
+  <si>
+    <t>for attiny across ground/vcc</t>
+  </si>
+  <si>
+    <t>6kohm resistor</t>
+  </si>
+  <si>
+    <t>http://ca.mouser.com/ProductDetail/KOA-Speer/RN732BTTD6001B25/?qs=sGAEpiMZZMu61qfTUdNhG9ZB66D1Zm68vK6lIlcdqUQ%3d</t>
+  </si>
+  <si>
+    <t>for op amp gain</t>
+  </si>
+  <si>
+    <t>shift register</t>
+  </si>
+  <si>
+    <t>http://ca.mouser.com/ProductDetail/Texas-Instruments/SN74HC164NSR/?qs=sGAEpiMZZMutXGli8Ay4kNJGVjTaPibHTsQo%252bdwnHbY%3d</t>
+  </si>
+  <si>
+    <t>for selecting op amp gain and button moffsets</t>
   </si>
   <si>
     <t>Total individual price</t>
@@ -232,9 +271,76 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2">
+      <c t="s" r="A2">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>0.072</v>
+      </c>
+      <c r="D2">
+        <v>0.048</v>
+      </c>
+      <c t="s" r="E2">
+        <v>9</v>
+      </c>
+      <c t="s" r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <f>B2*C2</f>
+        <v>0.216</v>
+      </c>
+      <c r="H2">
+        <f>D2*B2</f>
+        <v>0.144</v>
+      </c>
+    </row>
+    <row r="3">
+      <c t="s" r="A3">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c t="s" r="F3">
+        <v>12</v>
+      </c>
+      <c r="G3">
+        <f>B3*C3</f>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f>D3*B3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c t="s" r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0.312</v>
+      </c>
+      <c r="D4">
+        <v>0.274</v>
+      </c>
+      <c t="s" r="E4">
+        <v>14</v>
+      </c>
+      <c t="s" r="F4">
+        <v>15</v>
+      </c>
+    </row>
     <row r="5">
       <c t="s" r="A5">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -246,7 +352,7 @@
         <v>0.886</v>
       </c>
       <c t="s" r="E5">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G5">
         <f>B5*C5</f>
@@ -259,7 +365,7 @@
     </row>
     <row r="6">
       <c t="s" r="A6">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -271,7 +377,7 @@
         <v>2.02</v>
       </c>
       <c t="s" r="E6">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G6">
         <f>B6*C6</f>
@@ -284,63 +390,83 @@
     </row>
     <row r="7">
       <c t="s" r="A7">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>0.684</v>
+        <v>8.04</v>
       </c>
       <c r="D7">
-        <v>0.48</v>
+        <v>5.83</v>
       </c>
       <c t="s" s="1" r="E7">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G7">
         <f>B7*C7</f>
-        <v>1.368</v>
+        <v>8.04</v>
       </c>
       <c r="H7">
         <f>D7*B7</f>
-        <v>0.96</v>
+        <v>5.83</v>
       </c>
     </row>
     <row r="8">
       <c t="s" r="A8">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
       <c r="C8">
-        <v>0.432</v>
+        <v>0.756</v>
       </c>
       <c r="D8">
-        <v>0.365</v>
+        <v>0.662</v>
       </c>
       <c t="s" s="1" r="E8">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c t="s" r="F8">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="G8">
         <f>B8*C8</f>
-        <v>1.728</v>
+        <v>3.024</v>
       </c>
       <c r="H8">
         <f>D8*B8</f>
-        <v>1.46</v>
+        <v>2.648</v>
+      </c>
+    </row>
+    <row r="9">
+      <c t="s" r="A9">
+        <v>25</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0.66</v>
+      </c>
+      <c r="D9">
+        <v>0.588</v>
+      </c>
+      <c t="s" r="E9">
+        <v>26</v>
+      </c>
+      <c t="s" r="F9">
+        <v>27</v>
       </c>
     </row>
     <row r="10">
       <c t="s" r="A10">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <v>0.12</v>
@@ -349,23 +475,23 @@
         <v>0.09</v>
       </c>
       <c t="s" s="1" r="E10">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c t="s" r="F10">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="G10">
         <f>B10*C10</f>
-        <v>0.24</v>
+        <v>0.12</v>
       </c>
       <c r="H10">
         <f>D10*B10</f>
-        <v>0.18</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="13">
       <c t="s" r="A13">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -385,196 +511,181 @@
         <v>0.59</v>
       </c>
     </row>
+    <row r="14">
+      <c t="s" r="A14">
+        <v>32</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0.324</v>
+      </c>
+      <c r="D14">
+        <v>0.271</v>
+      </c>
+      <c t="s" r="E14">
+        <v>33</v>
+      </c>
+    </row>
     <row r="15">
       <c t="s" r="A15">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G15">
         <f>B15*C15</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H15">
         <f>D15*B15</f>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16">
       <c t="s" r="A16">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C16">
         <v>0.156</v>
       </c>
       <c r="D16">
-        <v>0.0049</v>
+        <v>0.049</v>
       </c>
       <c t="s" s="1" r="E16">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c t="s" r="F16">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="G16">
         <f>B16*C16</f>
-        <v>0.624</v>
+        <v>1.092</v>
       </c>
       <c r="H16">
         <f>D16*B16</f>
-        <v>0.0196</v>
+        <v>0.343</v>
       </c>
     </row>
     <row r="17">
       <c t="s" r="A17">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>0.744</v>
+        <v>0.732</v>
       </c>
       <c r="D17">
-        <v>0.51</v>
+        <v>0.467</v>
       </c>
       <c t="s" r="E17">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c t="s" r="F17">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="G17">
         <f>B17*C17</f>
-        <v>0.744</v>
+        <v>0.732</v>
       </c>
       <c r="H17">
         <f>D17*B17</f>
-        <v>0.51</v>
+        <v>0.467</v>
       </c>
     </row>
     <row r="18">
-      <c t="s" r="A18">
-        <v>28</v>
-      </c>
-      <c r="B18">
-        <v>2</v>
-      </c>
-      <c r="C18">
-        <v>0.564</v>
-      </c>
-      <c r="D18">
-        <v>0.184</v>
-      </c>
-      <c t="s" s="1" r="E18">
-        <v>29</v>
-      </c>
-      <c t="s" r="F18">
-        <v>30</v>
-      </c>
+      <c s="1" r="E18"/>
     </row>
     <row r="19">
       <c t="s" r="A19">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C19">
-        <v>0.888</v>
+        <v>0.072</v>
       </c>
       <c r="D19">
-        <v>0.513</v>
+        <v>0.043</v>
       </c>
       <c t="s" r="E19">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c t="s" r="F19">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="G19">
         <f>B19*C19</f>
-        <v>0.888</v>
+        <v>0.216</v>
       </c>
       <c r="H19">
         <f>D19*B19</f>
-        <v>0.513</v>
+        <v>0.129</v>
       </c>
     </row>
     <row r="20">
       <c t="s" r="A20">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
-      <c r="C20">
-        <v>0.072</v>
-      </c>
-      <c r="D20">
-        <v>0.048</v>
-      </c>
-      <c t="s" r="E20">
-        <v>34</v>
-      </c>
       <c t="s" r="F20">
-        <v>35</v>
-      </c>
-      <c r="G20">
-        <f>B20*C20</f>
-        <v>0.072</v>
-      </c>
-      <c r="H20">
-        <f>D20*B20</f>
-        <v>0.048</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21">
       <c t="s" r="A21">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21">
-        <v>0.072</v>
+        <v>0.6</v>
       </c>
       <c r="D21">
-        <v>0.048</v>
+        <v>0.432</v>
       </c>
       <c t="s" r="E21">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c t="s" r="F21">
-        <v>38</v>
-      </c>
-      <c r="G21">
-        <f>B21*C21</f>
-        <v>0.144</v>
-      </c>
-      <c r="H21">
-        <f>D21*B21</f>
-        <v>0.096</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22">
-      <c r="G22">
-        <f>B22*C22</f>
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <f>D22*B22</f>
-        <v>0</v>
+      <c t="s" r="A22">
+        <v>49</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>0.516</v>
+      </c>
+      <c r="D22">
+        <v>0.205</v>
+      </c>
+      <c t="s" r="E22">
+        <v>50</v>
+      </c>
+      <c t="s" r="F22">
+        <v>51</v>
       </c>
     </row>
     <row r="23">
@@ -593,20 +704,20 @@
         <v>0</v>
       </c>
       <c t="s" s="2" r="I24">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c t="s" s="2" r="K24">
-        <v>40</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25">
       <c r="I25">
         <f>SUM(G:G)</f>
-        <v>14.138</v>
+        <v>24.77</v>
       </c>
       <c r="K25">
         <f>SUM(H:H)</f>
-        <v>10.2826</v>
+        <v>19.147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>